<commit_message>
CRUD academicYear, CRUD user, update filehandler.js, update getById models
</commit_message>
<xml_diff>
--- a/src/fileExport/File_Export.xlsx
+++ b/src/fileExport/File_Export.xlsx
@@ -397,84 +397,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>code</v>
-      </c>
-      <c r="B1" t="str">
         <v>name</v>
-      </c>
-      <c r="C1" t="str">
-        <v>active</v>
-      </c>
-      <c r="D1" t="str">
-        <v>credit</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2">
-        <v>19089</v>
-      </c>
-      <c r="B2" t="str">
-        <v>Lap trinh huong doi tuong</v>
-      </c>
-      <c r="C2" t="b">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>4000000</v>
+      <c r="A2" t="str">
+        <v>.NET app 01</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3">
-        <v>19090</v>
-      </c>
-      <c r="B3" t="str">
-        <v>Lap trinh huong doi tuong 2</v>
-      </c>
-      <c r="C3" t="b">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>4000000</v>
+      <c r="A3" t="str">
+        <v>Mobile App</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4">
-        <v>19089</v>
-      </c>
-      <c r="B4" t="str">
-        <v>Lap trinh huong doi tuong</v>
-      </c>
-      <c r="C4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>4000000</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5">
-        <v>19090</v>
-      </c>
-      <c r="B5" t="str">
-        <v>Lap trinh huong doi tuong 2</v>
-      </c>
-      <c r="C5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>4000000</v>
+      <c r="A4" t="str">
+        <v xml:space="preserve">Web App </v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:A4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>